<commit_message>
Updated Test and Excel-Sheets
</commit_message>
<xml_diff>
--- a/Aufgaben/Aufgaben/normal_export.xlsx
+++ b/Aufgaben/Aufgaben/normal_export.xlsx
@@ -1,52 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinfu\source\repos\KI-Games-Ue\Aufgaben\Aufgaben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dokumente\KI-Games-Ue\Aufgaben\Aufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C93143A-70D1-4A98-BDFE-83EFD08E3663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618FD0D3-961E-483C-94C0-8E064AF31BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="normal_export" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">normal_export!$1:$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">normal_export!$A$1:$GR$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">normal_export!$1:$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">normal_export!$A$1:$GR$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,53 +512,54 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -585,41 +574,408 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="clusteredColumn" uniqueId="{CB480EA2-B67B-413D-A83D-6C30BBA8ED7A}">
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:binning intervalClosed="r" underflow="-10" overflow="10">
-              <cx:binSize val="1"/>
-            </cx:binning>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="0"/>
-        <cx:majorTickMarks type="cross"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Normalverteilung</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>normal_export!$B$4:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>normal_export!$C$4:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E0E5-46C4-A7D5-C0FBDB52E1DE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="2"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1769331167"/>
+        <c:axId val="1769326175"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1769331167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769326175"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1769326175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1769331167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,7 +1019,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -674,7 +1030,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -697,7 +1053,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -720,7 +1076,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -728,11 +1084,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -757,46 +1113,36 @@
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -811,8 +1157,10 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -820,12 +1168,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -835,13 +1180,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -860,16 +1205,18 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -940,6 +1287,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -971,8 +1324,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1027,7 +1380,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
@@ -1055,30 +1408,22 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat">
-        <a:solidFill>
-          <a:srgbClr val="D9D9D9"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -1094,7 +1439,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1110,7 +1455,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1124,7 +1469,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1157,7 +1502,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1166,6 +1511,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1174,87 +1525,45 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>240506</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>116679</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Chart 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96D103B7-92D3-4914-A7FB-331AEF2B0C4A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="240506" y="297654"/>
-              <a:ext cx="7531894" cy="4560095"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-DE" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
-Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0974B2FB-1E5E-42C3-A870-D530392F4B55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1549,615 +1858,804 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GR1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:GR24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:200" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
+    <row r="1" spans="1:200" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2">
         <v>-4</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>-7</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2">
         <v>2</v>
       </c>
-      <c r="F1" s="1">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1">
+      <c r="F1" s="2">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2">
         <v>4</v>
       </c>
-      <c r="H1" s="1">
-        <v>0</v>
-      </c>
-      <c r="I1" s="1">
+      <c r="H1" s="2">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2">
         <v>3</v>
       </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1">
+      <c r="J1" s="2">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2">
+        <v>1</v>
+      </c>
+      <c r="N1" s="2">
         <v>-2</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="2">
         <v>-2</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="2">
         <v>-2</v>
       </c>
-      <c r="Q1" s="1">
-        <v>0</v>
-      </c>
-      <c r="R1" s="1">
-        <v>0</v>
-      </c>
-      <c r="S1" s="1">
+      <c r="Q1" s="2">
+        <v>0</v>
+      </c>
+      <c r="R1" s="2">
+        <v>0</v>
+      </c>
+      <c r="S1" s="2">
         <v>-2</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1" s="2">
         <v>-4</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1" s="2">
         <v>-4</v>
       </c>
-      <c r="V1" s="1">
-        <v>0</v>
-      </c>
-      <c r="W1" s="1">
+      <c r="V1" s="2">
+        <v>0</v>
+      </c>
+      <c r="W1" s="2">
         <v>4</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X1" s="2">
         <v>-5</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y1" s="2">
         <v>-2</v>
       </c>
-      <c r="Z1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AA1" s="1">
+      <c r="Z1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AA1" s="2">
         <v>-6</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB1" s="2">
         <v>3</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC1" s="2">
         <v>-3</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD1" s="2">
         <v>2</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE1" s="2">
         <v>-4</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF1" s="2">
         <v>-6</v>
       </c>
-      <c r="AG1" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AI1" s="1">
+      <c r="AG1" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AI1" s="2">
         <v>-5</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AJ1" s="2">
         <v>5</v>
       </c>
-      <c r="AK1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AP1" s="1">
+      <c r="AK1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AM1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AO1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AP1" s="2">
         <v>-8</v>
       </c>
-      <c r="AQ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR1" s="1">
+      <c r="AQ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR1" s="2">
         <v>-4</v>
       </c>
-      <c r="AS1" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AU1" s="1">
+      <c r="AS1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AU1" s="2">
         <v>-5</v>
       </c>
-      <c r="AV1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AW1" s="1">
+      <c r="AV1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="AW1" s="2">
         <v>-2</v>
       </c>
-      <c r="AX1" s="1">
+      <c r="AX1" s="2">
         <v>4</v>
       </c>
-      <c r="AY1" s="1">
-        <v>1</v>
-      </c>
-      <c r="AZ1" s="1">
+      <c r="AY1" s="2">
+        <v>1</v>
+      </c>
+      <c r="AZ1" s="2">
         <v>-2</v>
       </c>
-      <c r="BA1" s="1">
-        <v>1</v>
-      </c>
-      <c r="BB1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD1" s="1">
+      <c r="BA1" s="2">
+        <v>1</v>
+      </c>
+      <c r="BB1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD1" s="2">
         <v>3</v>
       </c>
-      <c r="BE1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF1" s="1">
-        <v>1</v>
-      </c>
-      <c r="BG1" s="1">
+      <c r="BE1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF1" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG1" s="2">
         <v>-2</v>
       </c>
-      <c r="BH1" s="1">
+      <c r="BH1" s="2">
         <v>4</v>
       </c>
-      <c r="BI1" s="1">
+      <c r="BI1" s="2">
         <v>-2</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BJ1" s="2">
         <v>4</v>
       </c>
-      <c r="BK1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL1" s="1">
+      <c r="BK1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL1" s="2">
         <v>-2</v>
       </c>
-      <c r="BM1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="BN1" s="1">
+      <c r="BM1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="BN1" s="2">
         <v>3</v>
       </c>
-      <c r="BO1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP1" s="1">
-        <v>1</v>
-      </c>
-      <c r="BQ1" s="1">
+      <c r="BO1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BP1" s="2">
+        <v>1</v>
+      </c>
+      <c r="BQ1" s="2">
         <v>8</v>
       </c>
-      <c r="BR1" s="1">
-        <v>1</v>
-      </c>
-      <c r="BS1" s="1">
+      <c r="BR1" s="2">
+        <v>1</v>
+      </c>
+      <c r="BS1" s="2">
         <v>-3</v>
       </c>
-      <c r="BT1" s="1">
+      <c r="BT1" s="2">
         <v>4</v>
       </c>
-      <c r="BU1" s="1">
+      <c r="BU1" s="2">
         <v>3</v>
       </c>
-      <c r="BV1" s="1">
+      <c r="BV1" s="2">
         <v>2</v>
       </c>
-      <c r="BW1" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX1" s="1">
-        <v>1</v>
-      </c>
-      <c r="BY1" s="1">
+      <c r="BW1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BX1" s="2">
+        <v>1</v>
+      </c>
+      <c r="BY1" s="2">
         <v>-4</v>
       </c>
-      <c r="BZ1" s="1">
+      <c r="BZ1" s="2">
         <v>-3</v>
       </c>
-      <c r="CA1" s="1">
+      <c r="CA1" s="2">
         <v>-6</v>
       </c>
-      <c r="CB1" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC1" s="1">
+      <c r="CB1" s="2">
+        <v>0</v>
+      </c>
+      <c r="CC1" s="2">
         <v>2</v>
       </c>
-      <c r="CD1" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE1" s="1">
+      <c r="CD1" s="2">
+        <v>0</v>
+      </c>
+      <c r="CE1" s="2">
         <v>-5</v>
       </c>
-      <c r="CF1" s="1">
+      <c r="CF1" s="2">
         <v>5</v>
       </c>
-      <c r="CG1" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="CI1" s="1">
+      <c r="CG1" s="2">
+        <v>0</v>
+      </c>
+      <c r="CH1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="CI1" s="2">
         <v>2</v>
       </c>
-      <c r="CJ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK1" s="1">
-        <v>1</v>
-      </c>
-      <c r="CL1" s="1">
+      <c r="CJ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK1" s="2">
+        <v>1</v>
+      </c>
+      <c r="CL1" s="2">
         <v>2</v>
       </c>
-      <c r="CM1" s="1">
+      <c r="CM1" s="2">
         <v>-7</v>
       </c>
-      <c r="CN1" s="1">
+      <c r="CN1" s="2">
         <v>3</v>
       </c>
-      <c r="CO1" s="1">
+      <c r="CO1" s="2">
         <v>3</v>
       </c>
-      <c r="CP1" s="1">
+      <c r="CP1" s="2">
         <v>-3</v>
       </c>
-      <c r="CQ1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="CR1" s="1">
+      <c r="CQ1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="CR1" s="2">
         <v>-3</v>
       </c>
-      <c r="CS1" s="1">
-        <v>1</v>
-      </c>
-      <c r="CT1" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU1" s="1">
+      <c r="CS1" s="2">
+        <v>1</v>
+      </c>
+      <c r="CT1" s="2">
+        <v>0</v>
+      </c>
+      <c r="CU1" s="2">
         <v>-2</v>
       </c>
-      <c r="CV1" s="1">
+      <c r="CV1" s="2">
         <v>6</v>
       </c>
-      <c r="CW1" s="1">
+      <c r="CW1" s="2">
         <v>-6</v>
       </c>
-      <c r="CX1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="CY1" s="1">
+      <c r="CX1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="CY1" s="2">
         <v>3</v>
       </c>
-      <c r="CZ1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="DA1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DB1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DC1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DD1" s="1">
+      <c r="CZ1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="DA1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DB1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DC1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DD1" s="2">
         <v>-2</v>
       </c>
-      <c r="DE1" s="1">
+      <c r="DE1" s="2">
         <v>-3</v>
       </c>
-      <c r="DF1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DG1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DH1" s="1">
+      <c r="DF1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DG1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DH1" s="2">
         <v>4</v>
       </c>
-      <c r="DI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DJ1" s="1">
+      <c r="DI1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DJ1" s="2">
         <v>-4</v>
       </c>
-      <c r="DK1" s="1">
+      <c r="DK1" s="2">
         <v>-5</v>
       </c>
-      <c r="DL1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="DM1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DN1" s="1">
+      <c r="DL1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="DM1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DN1" s="2">
         <v>4</v>
       </c>
-      <c r="DO1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DP1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DQ1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DR1" s="1">
+      <c r="DO1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DP1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DQ1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DR1" s="2">
         <v>4</v>
       </c>
-      <c r="DS1" s="1">
+      <c r="DS1" s="2">
         <v>5</v>
       </c>
-      <c r="DT1" s="1">
-        <v>1</v>
-      </c>
-      <c r="DU1" s="1">
+      <c r="DT1" s="2">
+        <v>1</v>
+      </c>
+      <c r="DU1" s="2">
         <v>6</v>
       </c>
-      <c r="DV1" s="1">
-        <v>0</v>
-      </c>
-      <c r="DW1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="DX1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="DY1" s="1">
+      <c r="DV1" s="2">
+        <v>0</v>
+      </c>
+      <c r="DW1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="DX1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="DY1" s="2">
         <v>-3</v>
       </c>
-      <c r="DZ1" s="1">
+      <c r="DZ1" s="2">
         <v>2</v>
       </c>
-      <c r="EA1" s="1">
+      <c r="EA1" s="2">
         <v>-6</v>
       </c>
-      <c r="EB1" s="1">
-        <v>1</v>
-      </c>
-      <c r="EC1" s="1">
+      <c r="EB1" s="2">
+        <v>1</v>
+      </c>
+      <c r="EC1" s="2">
         <v>4</v>
       </c>
-      <c r="ED1" s="1">
+      <c r="ED1" s="2">
         <v>2</v>
       </c>
-      <c r="EE1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EF1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EG1" s="1">
+      <c r="EE1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EF1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EG1" s="2">
         <v>2</v>
       </c>
-      <c r="EH1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="EI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="EJ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EK1" s="1">
+      <c r="EH1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="EI1" s="2">
+        <v>1</v>
+      </c>
+      <c r="EJ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EK1" s="2">
         <v>7</v>
       </c>
-      <c r="EL1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EM1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="EN1" s="1">
-        <v>1</v>
-      </c>
-      <c r="EO1" s="1">
+      <c r="EL1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EM1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="EN1" s="2">
+        <v>1</v>
+      </c>
+      <c r="EO1" s="2">
         <v>4</v>
       </c>
-      <c r="EP1" s="1">
-        <v>1</v>
-      </c>
-      <c r="EQ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="ER1" s="1">
+      <c r="EP1" s="2">
+        <v>1</v>
+      </c>
+      <c r="EQ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="ER1" s="2">
         <v>-3</v>
       </c>
-      <c r="ES1" s="1">
+      <c r="ES1" s="2">
         <v>2</v>
       </c>
-      <c r="ET1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EU1" s="1">
-        <v>1</v>
-      </c>
-      <c r="EV1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="EW1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="EX1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EY1" s="1">
-        <v>0</v>
-      </c>
-      <c r="EZ1" s="1">
+      <c r="ET1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EU1" s="2">
+        <v>1</v>
+      </c>
+      <c r="EV1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="EW1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="EX1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EY1" s="2">
+        <v>0</v>
+      </c>
+      <c r="EZ1" s="2">
         <v>-7</v>
       </c>
-      <c r="FA1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FB1" s="1">
+      <c r="FA1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FB1" s="2">
         <v>-2</v>
       </c>
-      <c r="FC1" s="1">
+      <c r="FC1" s="2">
         <v>5</v>
       </c>
-      <c r="FD1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FE1" s="1">
+      <c r="FD1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE1" s="2">
         <v>3</v>
       </c>
-      <c r="FF1" s="1">
+      <c r="FF1" s="2">
         <v>-4</v>
       </c>
-      <c r="FG1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FH1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FJ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FK1" s="1">
+      <c r="FG1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FI1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FJ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FK1" s="2">
         <v>7</v>
       </c>
-      <c r="FL1" s="1">
+      <c r="FL1" s="2">
         <v>-7</v>
       </c>
-      <c r="FM1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="FN1" s="1">
+      <c r="FM1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="FN1" s="2">
         <v>5</v>
       </c>
-      <c r="FO1" s="1">
+      <c r="FO1" s="2">
         <v>4</v>
       </c>
-      <c r="FP1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FQ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FR1" s="1">
+      <c r="FP1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FQ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FR1" s="2">
         <v>2</v>
       </c>
-      <c r="FS1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FT1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FU1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FV1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="FW1" s="1">
-        <v>1</v>
-      </c>
-      <c r="FX1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="FY1" s="1">
-        <v>0</v>
-      </c>
-      <c r="FZ1" s="1">
+      <c r="FS1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FT1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FU1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FV1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="FW1" s="2">
+        <v>1</v>
+      </c>
+      <c r="FX1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="FY1" s="2">
+        <v>0</v>
+      </c>
+      <c r="FZ1" s="2">
         <v>4</v>
       </c>
-      <c r="GA1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="GB1" s="1">
+      <c r="GA1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="GB1" s="2">
         <v>6</v>
       </c>
-      <c r="GC1" s="1">
+      <c r="GC1" s="2">
         <v>2</v>
       </c>
-      <c r="GD1" s="1">
-        <v>0</v>
-      </c>
-      <c r="GE1" s="1">
+      <c r="GD1" s="2">
+        <v>0</v>
+      </c>
+      <c r="GE1" s="2">
         <v>-3</v>
       </c>
-      <c r="GF1" s="1">
+      <c r="GF1" s="2">
         <v>-2</v>
       </c>
-      <c r="GG1" s="1">
-        <v>1</v>
-      </c>
-      <c r="GH1" s="1">
+      <c r="GG1" s="2">
+        <v>1</v>
+      </c>
+      <c r="GH1" s="2">
         <v>-2</v>
       </c>
-      <c r="GI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="GJ1" s="1">
+      <c r="GI1" s="2">
+        <v>1</v>
+      </c>
+      <c r="GJ1" s="2">
         <v>-3</v>
       </c>
-      <c r="GK1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="GL1" s="1">
+      <c r="GK1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="GL1" s="2">
         <v>-3</v>
       </c>
-      <c r="GM1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="GN1" s="1">
+      <c r="GM1" s="2">
+        <v>-1</v>
+      </c>
+      <c r="GN1" s="2">
         <v>5</v>
       </c>
-      <c r="GO1" s="1">
+      <c r="GO1" s="2">
         <v>-2</v>
       </c>
-      <c r="GP1" s="1">
+      <c r="GP1" s="2">
         <v>2</v>
       </c>
-      <c r="GQ1" s="1">
-        <v>0</v>
-      </c>
-      <c r="GR1" s="1">
-        <v>-1</v>
+      <c r="GQ1" s="2">
+        <v>0</v>
+      </c>
+      <c r="GR1" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>-10</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIF($1:$1,B4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>-9</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C24" si="0">COUNTIF($1:$1,B5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>-8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>-7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>-5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>-4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>-3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
+        <v>-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:200" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="1">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="1">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>